<commit_message>
Sensible building cost numbers and tooltips
</commit_message>
<xml_diff>
--- a/Other Files/Design Excel.xlsx
+++ b/Other Files/Design Excel.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GitHub\CMP400\CMP400-Miniature-Kingdom\Other Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1438F4F-E4F2-49AD-8755-E2ACE7C8AED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2057A2D3-4284-462E-9AF7-C9884C56D165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9CC540EA-55F0-48B7-96A8-63FA4F1EDD42}"/>
+    <workbookView xWindow="28680" yWindow="45" windowWidth="29040" windowHeight="15840" xr2:uid="{9CC540EA-55F0-48B7-96A8-63FA4F1EDD42}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>Wood</t>
   </si>
@@ -118,6 +117,24 @@
   </si>
   <si>
     <t>Build Time 3 builders</t>
+  </si>
+  <si>
+    <t>2-2-2-2-2-1-1</t>
+  </si>
+  <si>
+    <t>Workers</t>
+  </si>
+  <si>
+    <t>Total work:</t>
+  </si>
+  <si>
+    <t>Build pattern:</t>
+  </si>
+  <si>
+    <t>Time Limit (mins)</t>
+  </si>
+  <si>
+    <t>Time Limit (secs)</t>
   </si>
 </sst>
 </file>
@@ -500,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71EC3720-B4B3-4445-81A2-AB93B5B49A8F}">
-  <dimension ref="B2:O19"/>
+  <dimension ref="B2:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,7 +582,7 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="H3">
         <v>5</v>
@@ -575,19 +592,19 @@
       </c>
       <c r="J3" s="1">
         <f>(C3/C17)+(E3/C18)+(D3/J17)+(F3/J18)+(G3/C19)</f>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="K3" s="1">
         <f t="shared" ref="K3:K9" si="0">J3+H3</f>
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="L3" s="1">
         <f>(J3 / ((1 + (I3))/2))+H3</f>
-        <v>9.7058823529411775</v>
+        <v>23.823529411764707</v>
       </c>
       <c r="M3" s="1">
         <f>(J3 / ((1 + (I3) + (I3 * I3))/3))+H3</f>
-        <v>10.479452054794521</v>
+        <v>26.917808219178081</v>
       </c>
       <c r="N3" s="1">
         <f>H3 / (1 +I3)</f>
@@ -603,7 +620,7 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="H4">
         <v>5</v>
@@ -613,19 +630,19 @@
       </c>
       <c r="J4" s="1">
         <f>(C4/C17)+(E4/C18)+(D4/J17)+(F4/J18)+(G4/C19)</f>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="K4" s="1">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="L4" s="1">
         <f t="shared" ref="L4:L9" si="1">(J4 / ((1 + (I4))/2))+H4</f>
-        <v>9.7058823529411775</v>
+        <v>23.823529411764707</v>
       </c>
       <c r="M4" s="1">
         <f t="shared" ref="M4:M9" si="2">(J4 / ((1 + (I4) + (I4 * I4))/3))+H4</f>
-        <v>10.479452054794521</v>
+        <v>26.917808219178081</v>
       </c>
       <c r="N4" s="1">
         <f t="shared" ref="N4:N9" si="3">H4 / (1 +I4)</f>
@@ -641,7 +658,7 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="H5">
         <v>5</v>
@@ -651,19 +668,19 @@
       </c>
       <c r="J5" s="1">
         <f>(C5/C17)+(E5/C18)+(D5/J17)+(F5/J18)+(G5/C19)</f>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="K5" s="1">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" si="1"/>
-        <v>9.7058823529411775</v>
+        <v>23.823529411764707</v>
       </c>
       <c r="M5" s="1">
         <f t="shared" si="2"/>
-        <v>10.479452054794521</v>
+        <v>26.917808219178081</v>
       </c>
       <c r="N5" s="1">
         <f t="shared" si="3"/>
@@ -679,40 +696,40 @@
         <v>7</v>
       </c>
       <c r="C6">
-        <v>325</v>
+        <v>450</v>
       </c>
       <c r="E6">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="H6">
-        <v>22.5</v>
+        <v>20</v>
       </c>
       <c r="I6">
         <v>0.7</v>
       </c>
       <c r="J6" s="1">
         <f>(C6/C17)+(E6/C18)+(D6/J17)+(F6/J18)+(G6/C19)</f>
-        <v>34.82352941176471</v>
+        <v>53.647058823529413</v>
       </c>
       <c r="K6" s="1">
         <f t="shared" si="0"/>
-        <v>57.32352941176471</v>
+        <v>73.64705882352942</v>
       </c>
       <c r="L6" s="1">
         <f>(J6 / ((1 + (I6))/2))+H6</f>
-        <v>63.468858131487899</v>
+        <v>83.114186851211073</v>
       </c>
       <c r="M6" s="1">
         <f t="shared" si="2"/>
-        <v>70.203464947622891</v>
+        <v>93.489121676067697</v>
       </c>
       <c r="N6" s="1">
         <f t="shared" si="3"/>
-        <v>13.23529411764706</v>
+        <v>11.764705882352942</v>
       </c>
       <c r="O6" s="1">
         <f t="shared" si="4"/>
-        <v>10.273972602739727</v>
+        <v>9.1324200913242013</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
@@ -720,40 +737,40 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>225</v>
+        <v>350</v>
       </c>
       <c r="E7">
-        <v>175</v>
+        <v>250</v>
       </c>
       <c r="H7">
-        <v>22.5</v>
+        <v>20</v>
       </c>
       <c r="I7">
         <v>0.7</v>
       </c>
       <c r="J7" s="1">
         <f>(C7/C17)+(E7/C18)+(D7/J17)+(F7/J18)+(G7/C19)</f>
-        <v>38.588235294117652</v>
+        <v>57.411764705882348</v>
       </c>
       <c r="K7" s="1">
         <f t="shared" si="0"/>
-        <v>61.088235294117652</v>
+        <v>77.411764705882348</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" si="1"/>
-        <v>67.897923875432525</v>
+        <v>87.543252595155707</v>
       </c>
       <c r="M7" s="1">
         <f t="shared" si="2"/>
-        <v>75.360596293311858</v>
+        <v>98.64625302175665</v>
       </c>
       <c r="N7" s="1">
         <f t="shared" si="3"/>
-        <v>13.23529411764706</v>
+        <v>11.764705882352942</v>
       </c>
       <c r="O7" s="1">
         <f t="shared" si="4"/>
-        <v>10.273972602739727</v>
+        <v>9.1324200913242013</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
@@ -761,10 +778,10 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="E8">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="H8">
         <v>15</v>
@@ -774,19 +791,19 @@
       </c>
       <c r="J8" s="1">
         <f>(C8/C17)+(E8/C18)+(D8/J17)+(F8/J18)+(G8/C19)</f>
-        <v>17.882352941176471</v>
+        <v>35.764705882352942</v>
       </c>
       <c r="K8" s="1">
         <f t="shared" si="0"/>
-        <v>32.882352941176471</v>
+        <v>50.764705882352942</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="1"/>
-        <v>36.038062283737027</v>
+        <v>57.076124567474054</v>
       </c>
       <c r="M8" s="1">
         <f t="shared" si="2"/>
-        <v>39.496373892022561</v>
+        <v>63.992747784045129</v>
       </c>
       <c r="N8" s="1">
         <f t="shared" si="3"/>
@@ -802,40 +819,40 @@
         <v>10</v>
       </c>
       <c r="D9">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="F9">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="H9">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="I9">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="J9" s="1">
         <f>(C9/C17)+(E9/C18)+(D9/J17)+(F9/J18)+(G9/C19)</f>
-        <v>280.74983839689719</v>
+        <v>421.12475759534584</v>
       </c>
       <c r="K9" s="1">
         <f t="shared" si="0"/>
-        <v>355.74983839689719</v>
+        <v>541.12475759534584</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" si="1"/>
-        <v>405.29392752576143</v>
+        <v>563.28921852141661</v>
       </c>
       <c r="M9" s="1">
         <f t="shared" si="2"/>
-        <v>459.58881972177699</v>
+        <v>586.18976855573339</v>
       </c>
       <c r="N9" s="1">
         <f t="shared" si="3"/>
-        <v>44.117647058823529</v>
+        <v>63.15789473684211</v>
       </c>
       <c r="O9" s="1">
         <f t="shared" si="4"/>
-        <v>34.246575342465754</v>
+        <v>44.280442804428041</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
@@ -843,11 +860,11 @@
         <v>12</v>
       </c>
       <c r="G10">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="J10" s="1">
         <f>(C10/C17)+(E10/C18)+(D10/J17)+(F10/J18)+(G10/C19)</f>
-        <v>200</v>
+        <v>300</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
@@ -870,7 +887,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>0</v>
       </c>
@@ -898,7 +915,7 @@
         <v>7.608695652173914</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>2</v>
       </c>
@@ -926,12 +943,59 @@
         <v>6.6969696969696964</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>11</v>
       </c>
       <c r="C19">
         <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N20" t="s">
+        <v>28</v>
+      </c>
+      <c r="O20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="N21" t="s">
+        <v>31</v>
+      </c>
+      <c r="O21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>30</v>
+      </c>
+      <c r="K22" t="s">
+        <v>27</v>
+      </c>
+      <c r="N22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O22">
+        <f>SUM(O21*60)</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>29</v>
+      </c>
+      <c r="K23">
+        <f>SUM((K3*2)+(K4*2)+(K5*2)+(K6*2)+(K7*2)+(K8)+(K9) + (J10))</f>
+        <v>1320.0071105365223</v>
+      </c>
+      <c r="N23" t="s">
+        <v>29</v>
+      </c>
+      <c r="O23">
+        <f>SUM(O20 * O22)</f>
+        <v>4800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>